<commit_message>
ran the code for product testing
</commit_message>
<xml_diff>
--- a/scraplingAdaptationHana/harristeeter/harris_teeter_price_compare/harris_teeter_pc.xlsx
+++ b/scraplingAdaptationHana/harristeeter/harris_teeter_price_compare/harris_teeter_pc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,10 +472,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9800895007</v>
+        <v>21718412169</v>
       </c>
       <c r="B2" t="n">
-        <v>5.49</v>
+        <v>8.989999999999998</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -498,15 +498,15 @@
         </is>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10900000185</v>
+        <v>846670000885</v>
       </c>
       <c r="B3" t="n">
-        <v>14.99</v>
+        <v>17.79</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -529,15 +529,15 @@
         </is>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10900000215</v>
+        <v>846670002353</v>
       </c>
       <c r="B4" t="n">
-        <v>6.49</v>
+        <v>12.99</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -560,15 +560,15 @@
         </is>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10900003308</v>
+        <v>13971010008</v>
       </c>
       <c r="B5" t="n">
-        <v>3.29</v>
+        <v>6.790000000000002</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -591,15 +591,15 @@
         </is>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10900743310</v>
+        <v>13971010015</v>
       </c>
       <c r="B6" t="n">
-        <v>4.99</v>
+        <v>6.790000000000002</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -622,15 +622,15 @@
         </is>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11115871324</v>
+        <v>13971021028</v>
       </c>
       <c r="B7" t="n">
-        <v>1.99</v>
+        <v>5.79</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -653,15 +653,15 @@
         </is>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13000006057</v>
+        <v>892234002048</v>
       </c>
       <c r="B8" t="n">
-        <v>7.49</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -684,15 +684,15 @@
         </is>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>13000007993</v>
+        <v>892234002017</v>
       </c>
       <c r="B9" t="n">
-        <v>4.29</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -715,15 +715,15 @@
         </is>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>13000008129</v>
+        <v>892234002000</v>
       </c>
       <c r="B10" t="n">
-        <v>2.49</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -742,15 +742,15 @@
         </is>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>13000008525</v>
+        <v>892234002024</v>
       </c>
       <c r="B11" t="n">
-        <v>2.29</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -769,15 +769,15 @@
         </is>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>13000008549</v>
+        <v>873204000028</v>
       </c>
       <c r="B12" t="n">
-        <v>2.99</v>
+        <v>6.989999999999999</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -800,15 +800,15 @@
         </is>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13000011105</v>
+        <v>873204001551</v>
       </c>
       <c r="B13" t="n">
-        <v>8.99</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -831,15 +831,15 @@
         </is>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13300204306</v>
+        <v>873204000905</v>
       </c>
       <c r="B14" t="n">
-        <v>2.99</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -862,15 +862,15 @@
         </is>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14800000344</v>
+        <v>73230008542</v>
       </c>
       <c r="B15" t="n">
-        <v>4.99</v>
+        <v>5.490000000000001</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -893,15 +893,15 @@
         </is>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14800002294</v>
+        <v>73230008511</v>
       </c>
       <c r="B16" t="n">
-        <v>5.29</v>
+        <v>4.765</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -924,15 +924,15 @@
         </is>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14800513240</v>
+        <v>73230008023</v>
       </c>
       <c r="B17" t="n">
-        <v>3.99</v>
+        <v>3.79</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -955,15 +955,15 @@
         </is>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16000106109</v>
+        <v>73230008573</v>
       </c>
       <c r="B18" t="n">
-        <v>6.99</v>
+        <v>10.99</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -986,15 +986,15 @@
         </is>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>16000107106</v>
+        <v>850006399086</v>
       </c>
       <c r="B19" t="n">
-        <v>3.99</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1017,15 +1017,15 @@
         </is>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16000122543</v>
+        <v>850006399055</v>
       </c>
       <c r="B20" t="n">
-        <v>6.99</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1048,15 +1048,15 @@
         </is>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>16000123991</v>
+        <v>850053667046</v>
       </c>
       <c r="B21" t="n">
-        <v>6.99</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1079,15 +1079,15 @@
         </is>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>16000124790</v>
+        <v>850053667008</v>
       </c>
       <c r="B22" t="n">
-        <v>6.99</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1110,15 +1110,15 @@
         </is>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>16000125063</v>
+        <v>850006399079</v>
       </c>
       <c r="B23" t="n">
-        <v>7.99</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1141,15 +1141,15 @@
         </is>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>16000275263</v>
+        <v>850006399727</v>
       </c>
       <c r="B24" t="n">
-        <v>6.49</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1172,15 +1172,15 @@
         </is>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>16000487727</v>
+        <v>8295667243</v>
       </c>
       <c r="B25" t="n">
-        <v>7.49</v>
+        <v>9.590000000000002</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1203,15 +1203,15 @@
         </is>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>16000487949</v>
+        <v>8295661036</v>
       </c>
       <c r="B26" t="n">
-        <v>6.49</v>
+        <v>5.990000000000001</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1234,15 +1234,15 @@
         </is>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>18000287949</v>
+        <v>8295661050</v>
       </c>
       <c r="B27" t="n">
-        <v>6.49</v>
+        <v>7.989999999999999</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1265,15 +1265,15 @@
         </is>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>18000817733</v>
+        <v>8295664853</v>
       </c>
       <c r="B28" t="n">
-        <v>6.29</v>
+        <v>32.99</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>18000817788</v>
+        <v>8295660107</v>
       </c>
       <c r="B29" t="n">
-        <v>6.29</v>
+        <v>9.289999999999997</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1313,15 +1313,15 @@
         </is>
       </c>
       <c r="G29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20113001534</v>
+        <v>747525200200</v>
       </c>
       <c r="B30" t="n">
-        <v>3.99</v>
+        <v>2.29</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1340,15 +1340,15 @@
         </is>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20735092767</v>
+        <v>747525200323</v>
       </c>
       <c r="B31" t="n">
-        <v>2.79</v>
+        <v>2.990000000000001</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1367,7 +1367,4343 @@
         </is>
       </c>
       <c r="G31" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>747525200644</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4.490000000000001</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0002073509286</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Turkey Hill® Lemonade</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>628110947154</v>
+      </c>
+      <c r="B33" t="n">
+        <v>7.790000000000002</v>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>628110947147</v>
+      </c>
+      <c r="B34" t="n">
+        <v>7.790000000000002</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0002100005439</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Kraft Sharp Cheddar Finely Shredded Cheese with 2% Milk</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>628110947123</v>
+      </c>
+      <c r="B35" t="n">
+        <v>7.790000000000002</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0002100005440</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Kraft Fat Free Cheddar Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>853883006252</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0002100005465</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Kraft Creamy Melt Mozzarella Cheese 8 oz</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>853883006030</v>
+      </c>
+      <c r="B37" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0002100005466</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Kraft Mexican Style Four Cheese Shredded Cheese With A Touch Of Philadelphia</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>853883006078</v>
+      </c>
+      <c r="B38" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>853883006047</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0002100005494</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Kraft Italian Five Cheese Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>853883006061</v>
+      </c>
+      <c r="B40" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0002100005495</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Kraft Mozzarella Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>853883006511</v>
+      </c>
+      <c r="B41" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0002100005496</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Kraft Mexican Style Four Cheese Blend Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>853883006412</v>
+      </c>
+      <c r="B42" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0002100005500</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Kraft Sharp Cheddar Finely Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>853883006504</v>
+      </c>
+      <c r="B43" t="n">
+        <v>5.948333333333334</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0002100005501</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Kraft Mild Cheddar Finely Shredded Cheese, 8 oz Bag</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>853883006566</v>
+      </c>
+      <c r="B44" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0002100005516</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Kraft Mozzarella Shredded Cheese Fine Cut</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>853883006436</v>
+      </c>
+      <c r="B45" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0002100005532</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Kraft Colby-Jack Shredded Cheese Fine Cut</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>853883006214</v>
+      </c>
+      <c r="B46" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0002100005534</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>USD 4.69</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Kraft Triple Cheddar Finely Shredded Cheese</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>853883006443</v>
+      </c>
+      <c r="B47" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0002100005536</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Kraft Deliciously Paired Cheddar &amp; Asadero Shredded Cheese with Taco Seasoning for Tacos</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>866558000004</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.789999999999999</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0002100060464</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>USD 5.99</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Kraft Singles American Sliced Cheese</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>850012039006</v>
+      </c>
+      <c r="B49" t="n">
+        <v>9.289999999999997</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0002100061215</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>USD 8.29</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Philadelphia Original Cream Cheese Spread</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>850012039013</v>
+      </c>
+      <c r="B50" t="n">
+        <v>9.289999999999997</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0002100061223</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>USD 4.39</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Philadelphia Original Cream Cheese</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>850012039044</v>
+      </c>
+      <c r="B51" t="n">
+        <v>9.289999999999997</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0002100061247</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>USD 4.39</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Philadelphia Reduced Fat Cream Cheese</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>850012039020</v>
+      </c>
+      <c r="B52" t="n">
+        <v>9.289999999999997</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0002100061531</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>USD 6.29</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Kraft Parmesan Grated Cheese</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>850012039037</v>
+      </c>
+      <c r="B53" t="n">
+        <v>9.289999999999997</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0002100061688</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>USD 7.39</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Philadelphia Original Cream Cheese Spread</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>865359000404</v>
+      </c>
+      <c r="B54" t="n">
+        <v>8.289999999999997</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0002100061984</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Philadelphia Original Whipped Cream Cheese Spread</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>78314111750</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0002100065883</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>USD 1.79</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Kraft Original Mac N Cheese Macaroni and Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>78314211757</v>
+      </c>
+      <c r="B56" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0002100065893</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>USD 4.79</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Velveeta Shells and Cheese Original Macaroni and Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>78314111002</v>
+      </c>
+      <c r="B57" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0002127310012</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Gunter Pure Clover Honey - 12 oz. - Pack of 3</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>78314112351</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9.489999999999998</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0002127360016</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Gunter's Pure Golden Honey</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>78314212358</v>
+      </c>
+      <c r="B59" t="n">
+        <v>9.489999999999998</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0002409401401</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>USD 4.19</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>De Cecco Potato Gnocchi</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>859750003867</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0002409407006</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>De Cecco Fettucine</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>859750003850</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0002409407007</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>De Cecco No. 7 Linguine</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>859750003287</v>
+      </c>
+      <c r="B62" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0002409407008</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>De Cecco Linguine Fini No 8 Pasta</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>859750003331</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0002409407009</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>De Cecco No 9 Angel Hair</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>859750003300</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0002409407011</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>De Cecco Thin Spaghetti 20X1 Lb</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>859750003294</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0002409407012</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>De Cecco No. 12 Spaghetti</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>859750003324</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0002409407024</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>USD 3.79</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>De Cecco Rigatoni No 24 Pasta</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>859750003317</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0002409407034</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>USD 3.79</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>De Cecco® Fusilli Pasta</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>859750003485</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0002409407041</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>USD 3.79</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>De Cecco Penne Rigate Pasta</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>850031185302</v>
+      </c>
+      <c r="B69" t="n">
+        <v>4.990000000000001</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0002409407050</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>De Cecco Conch Rigati</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>850031185296</v>
+      </c>
+      <c r="B70" t="n">
+        <v>4.990000000000001</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0002409407081</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>USD 3.19</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>De Cecco Enriched Macaroni Elbow Pasta</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>850031185319</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4.990000000000001</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0002409407087</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>De Cecco Cavatappi 1 LB. Pasta</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>859750003768</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0002409407091</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>De Cecco Orecchiette Pasta</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>850031185081</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0002409407093</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>USD 3.79</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>De Cecco Farfalle Bow Tie Pasta</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>859750003751</v>
+      </c>
+      <c r="B74" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0002460001003</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>USD 2.29</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Morton® Iodized Table Salt</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>850031185531</v>
+      </c>
+      <c r="B75" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0002484201121</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>USD 3.99</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Buitoni® Fettuccine Refrigerated Pasta Noodles</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>850031185548</v>
+      </c>
+      <c r="B76" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0002484207650</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>USD 9.99</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Buitoni® Mixed Cheese Tortellini Family Sized Pasta</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>75209824733</v>
+      </c>
+      <c r="B77" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0002484211211</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>USD 6.99</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Buitoni® Three Cheese Tortellini Refrigerated Pasta</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>75209827284</v>
+      </c>
+      <c r="B78" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0002484232111</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>USD 6.99</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Buitoni® Pesto with Basil Refrigerated Pasta Sauce</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>75209824948</v>
+      </c>
+      <c r="B79" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0002500004080</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Simply All Natural Orange Juice With Mango</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>75209824610</v>
+      </c>
+      <c r="B80" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0002500004082</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Simply Orange with Pineapple Juice</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>75209824931</v>
+      </c>
+      <c r="B81" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0002500004086</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Simply Lemonade With Strawberry All Natural Non-Gmo</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>75209827239</v>
+      </c>
+      <c r="B82" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0002500004088</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Simply Limeade Non-Gmo All Natural</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>75209824658</v>
+      </c>
+      <c r="B83" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0002500004400</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Simply High Pulp All Natural Orange Juice</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>75209825563</v>
+      </c>
+      <c r="B84" t="n">
+        <v>9.989999999999998</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0002500004483</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Simply Orange Medium Pulp Orange All Natural Juice With Calcium And Vitamin D</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>854401004132</v>
+      </c>
+      <c r="B85" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0002500004490</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Simply Lemonade With Raspberry All Natural Non-Gmo</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>854401004088</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0002500004496</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Simply All Natural Orange Juice With Calcium</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>854401004002</v>
+      </c>
+      <c r="B87" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0002500004498</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Simply Lemonade All Natural Non-Gmo</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>854401004026</v>
+      </c>
+      <c r="B88" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0002500005179</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Simply Fruit Punch All Natural Juice</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>854401004040</v>
+      </c>
+      <c r="B89" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0002500010000</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Simply Pulp Free All Natural Orange Juice</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>854401004286</v>
+      </c>
+      <c r="B90" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0002500010061</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Simply Light Lemonade All Natural Non-Gmo</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>877528000887</v>
+      </c>
+      <c r="B91" t="n">
+        <v>9.489999999999998</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0002500010071</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Simply Light Orange Pulp Free Orange All Natural Juice Non-Gmo</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>627843543831</v>
+      </c>
+      <c r="B92" t="n">
+        <v>10.29</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>0002500010211</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Simply Watermelon Fruit Juice Drink</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>850056882095</v>
+      </c>
+      <c r="B93" t="n">
+        <v>8.489999999999998</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0002500013405</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Simply® All Natural Pineapple Juice Drink</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>854758001037</v>
+      </c>
+      <c r="B94" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>0002500013642</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>USD 3.29</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Simply® Mango Juice Bottle</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>854758001112</v>
+      </c>
+      <c r="B95" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0002529300098</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>USD 4.49</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Silk Dairy Free Original Almond Milk Half Gallon</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>33674156919</v>
+      </c>
+      <c r="B96" t="n">
+        <v>22.99000000000001</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0002529300149</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>USD 4.49</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Silk Dairy Free Unsweeted Original Almond Milk Half Gallon</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>857416006245</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0002529360023</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Silk Dairy Free Organic Unsweetened Plain Soy Milk Half Gallon</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>850035919040</v>
+      </c>
+      <c r="B98" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0002529360027</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Silk Dairy Free Vanilla Soy Milk Half Gallon</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>853303007005</v>
+      </c>
+      <c r="B99" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0002529360039</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Silk Dairy Free Protein Original Soy Milk Half Gallon</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>198715314922</v>
+      </c>
+      <c r="B100" t="n">
+        <v>6.890000000000001</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0002700037800</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>USD 2.29</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Hunt's Fire Roasted Diced Tomatoes</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>198715162837</v>
+      </c>
+      <c r="B101" t="n">
+        <v>6.890000000000001</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0002700038040</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>USD 2.29</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Hunt’S Diced Tomatoes</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>77034013429</v>
+      </c>
+      <c r="B102" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>0002700038049</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>USD 2.29</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Hunt's No Salt Added Diced Tomatoes</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>77034013412</v>
+      </c>
+      <c r="B103" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0002700038143</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Hunt’S Tomato Ketchup</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>77034013405</v>
+      </c>
+      <c r="B104" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>0002700038811</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>USD 2.59</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Hunt’S Tomato Paste</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>77034013450</v>
+      </c>
+      <c r="B105" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0002700038815</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>USD 1.59</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Hunt’S Tomato Paste</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>77034011494</v>
+      </c>
+      <c r="B106" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0002700039005</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>USD 0.99</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Hunt's Tomato Sauce</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>77034011340</v>
+      </c>
+      <c r="B107" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0002700039007</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>USD 0.99</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Hunt's No Salt Added Tomato Sauce</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>77034011302</v>
+      </c>
+      <c r="B108" t="n">
+        <v>10.42333333333333</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0002700039014</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>USD 1.99</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Hunt's Tomato Sauce</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>25000044984</v>
+      </c>
+      <c r="B109" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0002800021580</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>USD 5.29</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Nestle Toll House Semi Sweet Chocolate Chips</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>25000040887</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0002840056463</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>USD 5.49</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Stacy's® Simply Naked® Baked Pita Chips Snacks</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>25000044908</v>
+      </c>
+      <c r="B111" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0003000001020</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>USD 4.19</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Quaker® Old Fashioned Oats</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>751217900965</v>
+      </c>
+      <c r="B112" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0003000001040</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>USD 7.19</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Quaker® Old Fashioned Oats</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>751217900934</v>
+      </c>
+      <c r="B113" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0003000001180</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>USD 4.19</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Quaker® Quick 1 Minute Oats</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>751217901023</v>
+      </c>
+      <c r="B114" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0003000001200</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>USD 7.19</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Quaker® Quick Oats</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>751217950038</v>
+      </c>
+      <c r="B115" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0003000065040</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company™ Original Pancake &amp; Waffle Mix</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>751217950007</v>
+      </c>
+      <c r="B116" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0003000065070</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company™ Complete Original Pancake &amp; Waffle Mix</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>751217940107</v>
+      </c>
+      <c r="B117" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0003000065300</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company Complete Pancake &amp; Waffle Mix Buttermilk</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>852375003014</v>
+      </c>
+      <c r="B118" t="n">
+        <v>7.489999999999999</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0003000065320</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company™ Buttermilk Pancake &amp; Waffle Mix 32 Oz</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>852375003007</v>
+      </c>
+      <c r="B119" t="n">
+        <v>7.489999999999999</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0003000065800</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>USD 4.99</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company Original Lite Syrup</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>28400611398</v>
+      </c>
+      <c r="B120" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0003000065940</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>USD 4.99</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company Butter Rich Syrup</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>28400718356</v>
+      </c>
+      <c r="B121" t="n">
+        <v>8.489999999999998</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0003000065970</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>USD 4.99</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Pearl Milling Company Syrup Original</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>28400718349</v>
+      </c>
+      <c r="B122" t="n">
+        <v>8.489999999999998</v>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>28400008488</v>
+      </c>
+      <c r="B123" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0003040079391</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>USD 5.59</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Angel Soft® Toilet Paper Mega Roll</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>28400008495</v>
+      </c>
+      <c r="B124" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0003040079414</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>USD 9.49</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Angel Soft® Toilet Paper Mega Roll</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>28400564632</v>
+      </c>
+      <c r="B125" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0003077204515</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>USD 7.79</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Charmin Essentials Strong Mega Roll Toilet Paper</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>28400564649</v>
+      </c>
+      <c r="B126" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0003077204537</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>USD 7.79</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Charmin Essentials Soft Mega Roll Toilet Paper</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>28400564656</v>
+      </c>
+      <c r="B127" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0003077205701</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>USD 13.99</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Bounty Select-A-Size Paper Towels Double Rolls</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>28400564663</v>
+      </c>
+      <c r="B128" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0003077205707</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>USD 8.99</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Bounty Select-A-Size Paper Towels Double Plus Rolls</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>803813101403</v>
+      </c>
+      <c r="B129" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>47281200422</v>
+      </c>
+      <c r="B130" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0003077215535</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>USD 7.49</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Cascade Platinum Dishwasher Pods Dishwasher Detergent Dish Detergent Soap Fresh</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>47281200354</v>
+      </c>
+      <c r="B131" t="n">
+        <v>6.489999999999999</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0003077215712</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>USD 13.99</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Bounty Paper Towels Select-A-Size White, 4 Double Rolls, 82 Sheets Per Roll</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>794522003501</v>
+      </c>
+      <c r="B132" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0003114200069</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>USD 15.99</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>BelGioioso® Sliced Fresh Mozzarella Cheese</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>794522003037</v>
+      </c>
+      <c r="B133" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>0003114200088</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>USD 8.99</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>BelGioioso Fresh Mozzarella Cheese</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>794522003051</v>
+      </c>
+      <c r="B134" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0003114200089</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>BelGioioso Fresh Mozzarella Cheese</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>794522003099</v>
+      </c>
+      <c r="B135" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0003114200480</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>USD 8.99</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>BelGioioso® Fresh Mozzarella Pearls Cheese</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>794522003563</v>
+      </c>
+      <c r="B136" t="n">
+        <v>5.490000000000001</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0003114200525</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>BelGioioso Fresh Mozzarella Cheese</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>794522001323</v>
+      </c>
+      <c r="B137" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>794522200344</v>
+      </c>
+      <c r="B138" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0003114235899</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>BelGioioso® Freshly Shaved Parmesan Cheese</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>794522200986</v>
+      </c>
+      <c r="B139" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0003114235900</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>BelGioioso® Freshly Grated Parmesan</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>794522200450</v>
+      </c>
+      <c r="B140" t="n">
+        <v>5.531666666666667</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0003114235902</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>BelGioioso® Parmesaon Cheese Freshly Shredded</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>794522703005</v>
+      </c>
+      <c r="B141" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>794522704002</v>
+      </c>
+      <c r="B142" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0003260102515</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Earthbound Farm Frozen Organic California-Style Blend</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>794522001422</v>
+      </c>
+      <c r="B143" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0003320001130</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>USD 0.99</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Arm &amp; Hammer Pure Baking Soda</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>794522002696</v>
+      </c>
+      <c r="B144" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0003485605092</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>USD 1.89</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Welch's Berries 'N Cherries Fruit Snacks</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>850044667024</v>
+      </c>
+      <c r="B145" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0003485605098</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>USD 1.89</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Welch's Mixed Fruit Fruit Snacks</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>850044667185</v>
+      </c>
+      <c r="B146" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0003500014108</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>USD 5.69</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Irish Spring Bar Soap Original Scent</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>850044667055</v>
+      </c>
+      <c r="B147" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0003500014116</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>USD 5.69</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Irish Spring 3-Pack Bar Soap Aloe Vera Scent</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>850044667048</v>
+      </c>
+      <c r="B148" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0003500044676</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Ajax Ultra Vinegar and Lime Scent Liquid Dish Soap</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>850044667130</v>
+      </c>
+      <c r="B149" t="n">
+        <v>2.765</v>
+      </c>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>850044667000</v>
+      </c>
+      <c r="B150" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0003600049995</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>USD 2.29</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Kleenex® Facial Tissues</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>810121960387</v>
+      </c>
+      <c r="B151" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>0003663200975</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>USD 7.49</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Danimals Strawberry Explosion &amp; Wild Watermelon Variety Pack Smoothies Bottle</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>90341232321</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0003663201039</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>USD 7.49</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Danimals® Non-GMO Strawberry Explosion &amp; Mixed Berry Smoothies</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>90341121212</v>
+      </c>
+      <c r="B153" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0003663202600</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Activia Low Fat Probiotic Strawberry Yogurt Cups</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>90341120048</v>
+      </c>
+      <c r="B154" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>90341543212</v>
+      </c>
+      <c r="B155" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>0003663203575</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Activia Probiotic Strawberry Dairy Drink Bottle</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>90341231157</v>
+      </c>
+      <c r="B156" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>90341200023</v>
+      </c>
+      <c r="B157" t="n">
+        <v>7.989999999999999</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>0003663207262</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>USD 6.99</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Stok® Extra Bold Unsweet Dark Roast Black Cold Brew Iced Coffee Carton</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>90341622009</v>
+      </c>
+      <c r="B158" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0003663207618</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>USD 6.99</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Stok® Unsweet Cold Brew Light Roast Black Iced Coffee Carton</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>90341620005</v>
+      </c>
+      <c r="B159" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0003700033840</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>USD 9.99</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Cascade Complete Fresh Scent Gel Dishwasher Detergent</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>90341623006</v>
+      </c>
+      <c r="B160" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>0003700034885</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>USD 4.99</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Bounty White Paper Napkins</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>90341626007</v>
+      </c>
+      <c r="B161" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0003746601643</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE Extra Creamy Milk Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>90341690008</v>
+      </c>
+      <c r="B162" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0003746601645</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE 85% Cocoa Dark Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>90341696000</v>
+      </c>
+      <c r="B163" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0003746601763</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE 70% Cocoa Dark Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>90341695003</v>
+      </c>
+      <c r="B164" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0003746602342</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE Intense Orange Dark Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>90341693009</v>
+      </c>
+      <c r="B165" t="n">
+        <v>6.989999999999999</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>0003746603941</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE Sea Salt Dark Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>856652006019</v>
+      </c>
+      <c r="B166" t="n">
+        <v>1.789999999999999</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0003746604269</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>USD 4.29</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Lindt EXCELLENCE 90% Cocoa Dark Chocolate Candy Bar</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>382431103629</v>
+      </c>
+      <c r="B167" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0003760011072</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>USD 3.39</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Skippy® Super Chunk® Extra Crunchy Peanut Butter Spread</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>382431102615</v>
+      </c>
+      <c r="B168" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>0003760011075</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>USD 3.39</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Skippy® Creamy Peanut Butter Spread</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>894410001098</v>
+      </c>
+      <c r="B169" t="n">
+        <v>5.990000000000001</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0003760013872</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>SPAM® Canned Luncheon Meat, Classic</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>814669010658</v>
+      </c>
+      <c r="B170" t="n">
+        <v>4.990000000000001</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0003800000110</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>USD 6.49</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Kellogg's® Corn Flakes Large Size Cereal</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>894410001258</v>
+      </c>
+      <c r="B171" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>0003800000120</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>USD 8.29</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Kellogg's® Corn Flakes Family Size Cereal</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>810029134798</v>
+      </c>
+      <c r="B172" t="n">
+        <v>3.990000000000002</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>0003800023145</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Kellogg's® Corn Flakes Giant Size Cereal</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>894410001944</v>
+      </c>
+      <c r="B173" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>0003800026985</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>USD 5.19</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Kellogg's® Special K Original Cereal</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>894410001937</v>
+      </c>
+      <c r="B174" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>0003800040260</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>USD 4.19</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Kellogg's® Eggo® Homestyle Homestyle Frozen Waffles</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>894410001012</v>
+      </c>
+      <c r="B175" t="n">
+        <v>2.990000000000001</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0003940001700</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>USD 1.79</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Bush's Chick Peas 16 oz</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>814669017640</v>
+      </c>
+      <c r="B176" t="n">
+        <v>2.490000000000001</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0003940001810</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>USD 1.79</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Bush's Pinto Beans 16 oz</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>0003940001870</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>USD 1.79</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Bush's Cannellini Beans 15.5 oz</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="G177" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>